<commit_message>
output weighted real estate metrics into excel with real estate score
</commit_message>
<xml_diff>
--- a/data/intermediate/metric_data.xlsx
+++ b/data/intermediate/metric_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t xml:space="preserve">cbsa</t>
   </si>
@@ -32,13 +32,19 @@
     <t xml:space="preserve">employ_change</t>
   </si>
   <si>
-    <t xml:space="preserve">med_rent_change</t>
+    <t xml:space="preserve">occ_rate2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rent_change</t>
   </si>
   <si>
     <t xml:space="preserve">income_to_homeprice</t>
   </si>
   <si>
-    <t xml:space="preserve">med_rent_to_income</t>
+    <t xml:space="preserve">rent_to_income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12060</t>
   </si>
   <si>
     <t xml:space="preserve">Atlanta-Sandy Springs-Alpharetta</t>
@@ -50,6 +56,9 @@
     <t xml:space="preserve">GA</t>
   </si>
   <si>
+    <t xml:space="preserve">12260</t>
+  </si>
+  <si>
     <t xml:space="preserve">Augusta-Richmond County</t>
   </si>
   <si>
@@ -59,6 +68,9 @@
     <t xml:space="preserve">GA-SC</t>
   </si>
   <si>
+    <t xml:space="preserve">16700</t>
+  </si>
+  <si>
     <t xml:space="preserve">Charleston-North Charleston</t>
   </si>
   <si>
@@ -68,6 +80,9 @@
     <t xml:space="preserve">SC</t>
   </si>
   <si>
+    <t xml:space="preserve">16740</t>
+  </si>
+  <si>
     <t xml:space="preserve">Charlotte-Concord-Gastonia</t>
   </si>
   <si>
@@ -77,21 +92,33 @@
     <t xml:space="preserve">NC-SC</t>
   </si>
   <si>
+    <t xml:space="preserve">16860</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chattanooga</t>
   </si>
   <si>
     <t xml:space="preserve">TN-GA</t>
   </si>
   <si>
+    <t xml:space="preserve">17820</t>
+  </si>
+  <si>
     <t xml:space="preserve">Colorado Springs</t>
   </si>
   <si>
     <t xml:space="preserve">CO</t>
   </si>
   <si>
+    <t xml:space="preserve">17900</t>
+  </si>
+  <si>
     <t xml:space="preserve">Columbia</t>
   </si>
   <si>
+    <t xml:space="preserve">19780</t>
+  </si>
+  <si>
     <t xml:space="preserve">Des Moines-West Des Moines</t>
   </si>
   <si>
@@ -101,30 +128,45 @@
     <t xml:space="preserve">IA</t>
   </si>
   <si>
+    <t xml:space="preserve">22180</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fayetteville</t>
   </si>
   <si>
     <t xml:space="preserve">NC</t>
   </si>
   <si>
+    <t xml:space="preserve">22220</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fayetteville-Springdale-Rogers</t>
   </si>
   <si>
     <t xml:space="preserve">AR</t>
   </si>
   <si>
+    <t xml:space="preserve">24860</t>
+  </si>
+  <si>
     <t xml:space="preserve">Greenville-Anderson</t>
   </si>
   <si>
     <t xml:space="preserve">Greenville</t>
   </si>
   <si>
+    <t xml:space="preserve">26620</t>
+  </si>
+  <si>
     <t xml:space="preserve">Huntsville</t>
   </si>
   <si>
     <t xml:space="preserve">AL</t>
   </si>
   <si>
+    <t xml:space="preserve">26900</t>
+  </si>
+  <si>
     <t xml:space="preserve">Indianapolis-Carmel-Anderson</t>
   </si>
   <si>
@@ -134,12 +176,18 @@
     <t xml:space="preserve">IN</t>
   </si>
   <si>
+    <t xml:space="preserve">28940</t>
+  </si>
+  <si>
     <t xml:space="preserve">Knoxville</t>
   </si>
   <si>
     <t xml:space="preserve">TN</t>
   </si>
   <si>
+    <t xml:space="preserve">29460</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lakeland-Winter Haven</t>
   </si>
   <si>
@@ -149,6 +197,9 @@
     <t xml:space="preserve">FL</t>
   </si>
   <si>
+    <t xml:space="preserve">32580</t>
+  </si>
+  <si>
     <t xml:space="preserve">McAllen-Edinburg-Mission</t>
   </si>
   <si>
@@ -158,6 +209,9 @@
     <t xml:space="preserve">TX</t>
   </si>
   <si>
+    <t xml:space="preserve">34820</t>
+  </si>
+  <si>
     <t xml:space="preserve">Myrtle Beach-Conway-North Myrtle Beach</t>
   </si>
   <si>
@@ -167,36 +221,54 @@
     <t xml:space="preserve">SC-NC</t>
   </si>
   <si>
+    <t xml:space="preserve">34980</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nashville-Davidson--Murfreesboro--Franklin</t>
   </si>
   <si>
     <t xml:space="preserve">Nashville</t>
   </si>
   <si>
+    <t xml:space="preserve">35840</t>
+  </si>
+  <si>
     <t xml:space="preserve">North Port-Sarasota-Bradenton</t>
   </si>
   <si>
     <t xml:space="preserve">Sarasota</t>
   </si>
   <si>
+    <t xml:space="preserve">36420</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oklahoma City</t>
   </si>
   <si>
     <t xml:space="preserve">OK</t>
   </si>
   <si>
+    <t xml:space="preserve">37340</t>
+  </si>
+  <si>
     <t xml:space="preserve">Palm Bay-Melbourne-Titusville</t>
   </si>
   <si>
     <t xml:space="preserve">Palm Bay</t>
   </si>
   <si>
+    <t xml:space="preserve">37860</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pensacola-Ferry Pass-Brent</t>
   </si>
   <si>
     <t xml:space="preserve">Pensacola</t>
   </si>
   <si>
+    <t xml:space="preserve">38860</t>
+  </si>
+  <si>
     <t xml:space="preserve">Portland-South Portland</t>
   </si>
   <si>
@@ -206,27 +278,42 @@
     <t xml:space="preserve">ME</t>
   </si>
   <si>
+    <t xml:space="preserve">38940</t>
+  </si>
+  <si>
     <t xml:space="preserve">Port St. Lucie</t>
   </si>
   <si>
+    <t xml:space="preserve">39580</t>
+  </si>
+  <si>
     <t xml:space="preserve">Raleigh-Cary</t>
   </si>
   <si>
     <t xml:space="preserve">Raleigh</t>
   </si>
   <si>
+    <t xml:space="preserve">40060</t>
+  </si>
+  <si>
     <t xml:space="preserve">Richmond</t>
   </si>
   <si>
     <t xml:space="preserve">VA</t>
   </si>
   <si>
+    <t xml:space="preserve">41700</t>
+  </si>
+  <si>
     <t xml:space="preserve">San Antonio-New Braunfels</t>
   </si>
   <si>
     <t xml:space="preserve">San Antonio</t>
   </si>
   <si>
+    <t xml:space="preserve">44060</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spokane-Spokane Valley</t>
   </si>
   <si>
@@ -234,6 +321,9 @@
   </si>
   <si>
     <t xml:space="preserve">WA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49180</t>
   </si>
   <si>
     <t xml:space="preserve">Winston-Salem</t>
@@ -599,19 +689,22 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>12060</v>
+      <c r="A2" t="s">
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" t="n">
         <v>0.703</v>
@@ -620,27 +713,30 @@
         <v>3.0655</v>
       </c>
       <c r="G2" t="n">
+        <v>95.3</v>
+      </c>
+      <c r="H2" t="n">
         <v>8.8809946714032</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0.244605926860025</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0.174148397324363</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>12260</v>
+      <c r="A3" t="s">
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E3" t="n">
         <v>0.689</v>
@@ -649,27 +745,30 @@
         <v>1.8641</v>
       </c>
       <c r="G3" t="n">
+        <v>95.2</v>
+      </c>
+      <c r="H3" t="n">
         <v>11.3428943937419</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0.150626332622601</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>0.162859417853667</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>16700</v>
+      <c r="A4" t="s">
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E4" t="n">
         <v>1.257</v>
@@ -678,27 +777,30 @@
         <v>2.3757</v>
       </c>
       <c r="G4" t="n">
+        <v>95.1</v>
+      </c>
+      <c r="H4" t="n">
         <v>14.1125541125541</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>0.205362891838464</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.190596680372392</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>16740</v>
+      <c r="A5" t="s">
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E5" t="n">
         <v>1.175</v>
@@ -707,27 +809,30 @@
         <v>2.6157</v>
       </c>
       <c r="G5" t="n">
+        <v>95.4</v>
+      </c>
+      <c r="H5" t="n">
         <v>0.917431192660551</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>0.278264786525656</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>0.184119029855999</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>16860</v>
+      <c r="A6" t="s">
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E6" t="n">
         <v>0.717</v>
@@ -736,27 +841,30 @@
         <v>2.961</v>
       </c>
       <c r="G6" t="n">
+        <v>96.27</v>
+      </c>
+      <c r="H6" t="n">
         <v>6.83646112600536</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>0.144109494109494</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>0.143496032700168</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>17820</v>
+      <c r="A7" t="s">
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E7" t="n">
         <v>0.822</v>
@@ -765,27 +873,30 @@
         <v>1.3</v>
       </c>
       <c r="G7" t="n">
+        <v>96.2</v>
+      </c>
+      <c r="H7" t="n">
         <v>8.03484995159729</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>0.338825042881647</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>0.156883590249829</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>17900</v>
+      <c r="A8" t="s">
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E8" t="n">
         <v>0.901</v>
@@ -794,27 +905,30 @@
         <v>1.4736</v>
       </c>
       <c r="G8" t="n">
+        <v>94.9</v>
+      </c>
+      <c r="H8" t="n">
         <v>2.30010952902519</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>0.225457010069713</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>0.188205383677186</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>19780</v>
+      <c r="A9" t="s">
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="E9" t="n">
         <v>1.168</v>
@@ -823,27 +937,30 @@
         <v>1.3035</v>
       </c>
       <c r="G9" t="n">
+        <v>94.8</v>
+      </c>
+      <c r="H9" t="n">
         <v>4.46998722860792</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>0.390979978925184</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>0.126617076326003</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>22180</v>
+      <c r="A10" t="s">
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E10" t="n">
         <v>0.814</v>
@@ -852,27 +969,30 @@
         <v>2.3854</v>
       </c>
       <c r="G10" t="n">
+        <v>95</v>
+      </c>
+      <c r="H10" t="n">
         <v>5.13141426783479</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>0.20290191740413</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>0.174241735875116</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>22220</v>
+      <c r="A11" t="s">
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E11" t="n">
         <v>2.028</v>
@@ -881,27 +1001,30 @@
         <v>1.7117</v>
       </c>
       <c r="G11" t="n">
+        <v>96.65</v>
+      </c>
+      <c r="H11" t="n">
         <v>11.8181818181818</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>0.25713722680043</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>0.110357127927878</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>24860</v>
+      <c r="A12" t="s">
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E12" t="n">
         <v>1.141</v>
@@ -910,27 +1033,30 @@
         <v>2.1585</v>
       </c>
       <c r="G12" t="n">
+        <v>95.3</v>
+      </c>
+      <c r="H12" t="n">
         <v>5.68561872909699</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>0.222057774607703</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>0.172874006263551</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>26620</v>
+      <c r="A13" t="s">
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E13" t="n">
         <v>1.763</v>
@@ -939,27 +1065,30 @@
         <v>2.565</v>
       </c>
       <c r="G13" t="n">
+        <v>96.64</v>
+      </c>
+      <c r="H13" t="n">
         <v>11.4401076716016</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>0.295443378119002</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>0.115847874952899</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>26900</v>
+      <c r="A14" t="s">
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="E14" t="n">
         <v>0.62</v>
@@ -968,27 +1097,30 @@
         <v>3.4493</v>
       </c>
       <c r="G14" t="n">
+        <v>95.1</v>
+      </c>
+      <c r="H14" t="n">
         <v>0.240673886883273</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>0.251698924731183</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>0.142002734107997</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>28940</v>
+      <c r="A15" t="s">
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E15" t="n">
         <v>1.337</v>
@@ -997,27 +1129,30 @@
         <v>2.8531</v>
       </c>
       <c r="G15" t="n">
+        <v>97.71</v>
+      </c>
+      <c r="H15" t="n">
         <v>9.84654731457801</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>0.231822222222222</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>0.149923312883436</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>29460</v>
+      <c r="A16" t="s">
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="E16" t="n">
         <v>3.33</v>
@@ -1026,27 +1161,30 @@
         <v>4.7599</v>
       </c>
       <c r="G16" t="n">
+        <v>97.19</v>
+      </c>
+      <c r="H16" t="n">
         <v>5.47147846332945</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>0.191765306122449</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>0.182834033948811</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>32580</v>
+      <c r="A17" t="s">
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="E17" t="n">
         <v>0.935</v>
@@ -1055,27 +1193,30 @@
         <v>2.6371</v>
       </c>
       <c r="G17" t="n">
+        <v>96.6</v>
+      </c>
+      <c r="H17" t="n">
         <v>10.983606557377</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>0.128234620886981</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>0.163327234593244</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>34820</v>
+      <c r="A18" t="s">
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="E18" t="n">
         <v>3.705</v>
@@ -1084,27 +1225,30 @@
         <v>3.3864</v>
       </c>
       <c r="G18" t="n">
+        <v>96.4</v>
+      </c>
+      <c r="H18" t="n">
         <v>20.6683168316832</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>0.145859259259259</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>0.164135899649586</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>34980</v>
+      <c r="A19" t="s">
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E19" t="n">
         <v>0.859</v>
@@ -1113,27 +1257,30 @@
         <v>3.6637</v>
       </c>
       <c r="G19" t="n">
+        <v>94.77</v>
+      </c>
+      <c r="H19" t="n">
         <v>7.36086175942549</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>0.374485066941298</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>0.183815744242008</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>35840</v>
+      <c r="A20" t="s">
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="E20" t="n">
         <v>2.706</v>
@@ -1142,27 +1289,30 @@
         <v>3.7887</v>
       </c>
       <c r="G20" t="n">
+        <v>96.23</v>
+      </c>
+      <c r="H20" t="n">
         <v>8.7360594795539</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>0.229819672131148</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>0.184207147442756</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>36420</v>
+      <c r="A21" t="s">
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="E21" t="n">
         <v>0.906</v>
@@ -1171,27 +1321,30 @@
         <v>2.703</v>
       </c>
       <c r="G21" t="n">
+        <v>93.7</v>
+      </c>
+      <c r="H21" t="n">
         <v>1.14649681528662</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>0.219982206405694</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>0.152390196554234</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>37340</v>
+      <c r="A22" t="s">
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="E22" t="n">
         <v>1.418</v>
@@ -1200,27 +1353,30 @@
         <v>3.3806</v>
       </c>
       <c r="G22" t="n">
+        <v>96.64</v>
+      </c>
+      <c r="H22" t="n">
         <v>7.17213114754098</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>0.196786144578313</v>
       </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
         <v>0.179266220746024</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>37860</v>
+      <c r="A23" t="s">
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" t="s">
         <v>60</v>
-      </c>
-      <c r="D23" t="s">
-        <v>44</v>
       </c>
       <c r="E23" t="n">
         <v>0.944</v>
@@ -1229,27 +1385,30 @@
         <v>2.7199</v>
       </c>
       <c r="G23" t="n">
+        <v>96.8</v>
+      </c>
+      <c r="H23" t="n">
         <v>4.77247502774695</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>0.155171011719684</v>
       </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
         <v>0.166653821847496</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>38860</v>
+      <c r="A24" t="s">
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="E24" t="n">
         <v>0.87</v>
@@ -1258,27 +1417,30 @@
         <v>3.5695</v>
       </c>
       <c r="G24" t="n">
+        <v>98.86</v>
+      </c>
+      <c r="H24" t="n">
         <v>10.8108108108108</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>0.199994908350306</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
         <v>0.19781562667074</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>38940</v>
+      <c r="A25" t="s">
+        <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="E25" t="n">
         <v>2.801</v>
@@ -1287,27 +1449,30 @@
         <v>0.9179</v>
       </c>
       <c r="G25" t="n">
+        <v>94.4</v>
+      </c>
+      <c r="H25" t="n">
         <v>6.00600600600601</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>0.18602975495916</v>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
         <v>0.187985134308698</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>39580</v>
+      <c r="A26" t="s">
+        <v>90</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E26" t="n">
         <v>1.985</v>
@@ -1316,27 +1481,30 @@
         <v>2.3456</v>
       </c>
       <c r="G26" t="n">
+        <v>95.5</v>
+      </c>
+      <c r="H26" t="n">
         <v>1.85185185185185</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>0.292936126373626</v>
       </c>
-      <c r="I26" t="n">
+      <c r="J26" t="n">
         <v>0.159525456314549</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>40060</v>
+      <c r="A27" t="s">
+        <v>93</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="E27" t="n">
         <v>0.633</v>
@@ -1345,27 +1513,30 @@
         <v>2.6413</v>
       </c>
       <c r="G27" t="n">
+        <v>95.75</v>
+      </c>
+      <c r="H27" t="n">
         <v>2.00364298724954</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>0.194061763936142</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>0.177691467411094</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>41700</v>
+      <c r="A28" t="s">
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="E28" t="n">
         <v>1.368</v>
@@ -1374,27 +1545,30 @@
         <v>2.3486</v>
       </c>
       <c r="G28" t="n">
+        <v>96.2</v>
+      </c>
+      <c r="H28" t="n">
         <v>5.91233435270133</v>
       </c>
-      <c r="H28" t="n">
+      <c r="I28" t="n">
         <v>0.283425297113752</v>
       </c>
-      <c r="I28" t="n">
+      <c r="J28" t="n">
         <v>0.176293523025084</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>44060</v>
+      <c r="A29" t="s">
+        <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="E29" t="n">
         <v>1.056</v>
@@ -1403,27 +1577,30 @@
         <v>3.129</v>
       </c>
       <c r="G29" t="n">
+        <v>98.3</v>
+      </c>
+      <c r="H29" t="n">
         <v>2.68292682926829</v>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>0.229143559143559</v>
       </c>
-      <c r="I29" t="n">
+      <c r="J29" t="n">
         <v>0.150728367262534</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>49180</v>
+      <c r="A30" t="s">
+        <v>103</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="D30" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E30" t="n">
         <v>0.749</v>
@@ -1432,12 +1609,15 @@
         <v>2.4865</v>
       </c>
       <c r="G30" t="n">
+        <v>95.9</v>
+      </c>
+      <c r="H30" t="n">
         <v>-1.26404494382022</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>0.221590733590734</v>
       </c>
-      <c r="I30" t="n">
+      <c r="J30" t="n">
         <v>0.148870922776694</v>
       </c>
     </row>

</xml_diff>

<commit_message>
output reopt data in excel
</commit_message>
<xml_diff>
--- a/data/intermediate/metric_data.xlsx
+++ b/data/intermediate/metric_data.xlsx
@@ -7,26 +7,30 @@
   </bookViews>
   <sheets>
     <sheet name="real_estate_metrics" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="testn_landlord_metrics" r:id="rId5" sheetId="2"/>
+    <sheet name="n_real_estate_metrics" r:id="rId6" sheetId="3"/>
+    <sheet name="landlord_metrics" r:id="rId7" sheetId="4"/>
+    <sheet name="n_climate_risk_metrics" r:id="rId8" sheetId="5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="318">
   <si>
     <t xml:space="preserve">cbsa</t>
   </si>
   <si>
+    <t xml:space="preserve">anchor_city</t>
+  </si>
+  <si>
     <t xml:space="preserve">msa</t>
   </si>
   <si>
-    <t xml:space="preserve">anchor_city</t>
-  </si>
-  <si>
     <t xml:space="preserve">state.x</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_change</t>
+    <t xml:space="preserve">pop_growth</t>
   </si>
   <si>
     <t xml:space="preserve">employ_change</t>
@@ -47,48 +51,48 @@
     <t xml:space="preserve">12060</t>
   </si>
   <si>
+    <t xml:space="preserve">Atlanta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Atlanta-Sandy Springs-Alpharetta</t>
   </si>
   <si>
-    <t xml:space="preserve">Atlanta</t>
-  </si>
-  <si>
     <t xml:space="preserve">GA</t>
   </si>
   <si>
     <t xml:space="preserve">12260</t>
   </si>
   <si>
+    <t xml:space="preserve">Augusta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Augusta-Richmond County</t>
   </si>
   <si>
-    <t xml:space="preserve">Augusta</t>
-  </si>
-  <si>
     <t xml:space="preserve">GA-SC</t>
   </si>
   <si>
     <t xml:space="preserve">16700</t>
   </si>
   <si>
+    <t xml:space="preserve">Charleston</t>
+  </si>
+  <si>
     <t xml:space="preserve">Charleston-North Charleston</t>
   </si>
   <si>
-    <t xml:space="preserve">Charleston</t>
-  </si>
-  <si>
     <t xml:space="preserve">SC</t>
   </si>
   <si>
     <t xml:space="preserve">16740</t>
   </si>
   <si>
+    <t xml:space="preserve">Charlotte</t>
+  </si>
+  <si>
     <t xml:space="preserve">Charlotte-Concord-Gastonia</t>
   </si>
   <si>
-    <t xml:space="preserve">Charlotte</t>
-  </si>
-  <si>
     <t xml:space="preserve">NC-SC</t>
   </si>
   <si>
@@ -119,12 +123,12 @@
     <t xml:space="preserve">19780</t>
   </si>
   <si>
+    <t xml:space="preserve">Des Moines</t>
+  </si>
+  <si>
     <t xml:space="preserve">Des Moines-West Des Moines</t>
   </si>
   <si>
-    <t xml:space="preserve">Des Moines</t>
-  </si>
-  <si>
     <t xml:space="preserve">IA</t>
   </si>
   <si>
@@ -149,12 +153,12 @@
     <t xml:space="preserve">24860</t>
   </si>
   <si>
+    <t xml:space="preserve">Greenville</t>
+  </si>
+  <si>
     <t xml:space="preserve">Greenville-Anderson</t>
   </si>
   <si>
-    <t xml:space="preserve">Greenville</t>
-  </si>
-  <si>
     <t xml:space="preserve">26620</t>
   </si>
   <si>
@@ -167,12 +171,12 @@
     <t xml:space="preserve">26900</t>
   </si>
   <si>
+    <t xml:space="preserve">Indianapolis</t>
+  </si>
+  <si>
     <t xml:space="preserve">Indianapolis-Carmel-Anderson</t>
   </si>
   <si>
-    <t xml:space="preserve">Indianapolis</t>
-  </si>
-  <si>
     <t xml:space="preserve">IN</t>
   </si>
   <si>
@@ -188,57 +192,57 @@
     <t xml:space="preserve">29460</t>
   </si>
   <si>
+    <t xml:space="preserve">Lakeland</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lakeland-Winter Haven</t>
   </si>
   <si>
-    <t xml:space="preserve">Lakeland</t>
-  </si>
-  <si>
     <t xml:space="preserve">FL</t>
   </si>
   <si>
     <t xml:space="preserve">32580</t>
   </si>
   <si>
+    <t xml:space="preserve">McAllen</t>
+  </si>
+  <si>
     <t xml:space="preserve">McAllen-Edinburg-Mission</t>
   </si>
   <si>
-    <t xml:space="preserve">McAllen</t>
-  </si>
-  <si>
     <t xml:space="preserve">TX</t>
   </si>
   <si>
     <t xml:space="preserve">34820</t>
   </si>
   <si>
+    <t xml:space="preserve">Myrtle Beach</t>
+  </si>
+  <si>
     <t xml:space="preserve">Myrtle Beach-Conway-North Myrtle Beach</t>
   </si>
   <si>
-    <t xml:space="preserve">Myrtle Beach</t>
-  </si>
-  <si>
     <t xml:space="preserve">SC-NC</t>
   </si>
   <si>
     <t xml:space="preserve">34980</t>
   </si>
   <si>
+    <t xml:space="preserve">Nashville</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nashville-Davidson--Murfreesboro--Franklin</t>
   </si>
   <si>
-    <t xml:space="preserve">Nashville</t>
-  </si>
-  <si>
     <t xml:space="preserve">35840</t>
   </si>
   <si>
+    <t xml:space="preserve">Sarasota</t>
+  </si>
+  <si>
     <t xml:space="preserve">North Port-Sarasota-Bradenton</t>
   </si>
   <si>
-    <t xml:space="preserve">Sarasota</t>
-  </si>
-  <si>
     <t xml:space="preserve">36420</t>
   </si>
   <si>
@@ -251,30 +255,30 @@
     <t xml:space="preserve">37340</t>
   </si>
   <si>
+    <t xml:space="preserve">Palm Bay</t>
+  </si>
+  <si>
     <t xml:space="preserve">Palm Bay-Melbourne-Titusville</t>
   </si>
   <si>
-    <t xml:space="preserve">Palm Bay</t>
-  </si>
-  <si>
     <t xml:space="preserve">37860</t>
   </si>
   <si>
+    <t xml:space="preserve">Pensacola</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pensacola-Ferry Pass-Brent</t>
   </si>
   <si>
-    <t xml:space="preserve">Pensacola</t>
-  </si>
-  <si>
     <t xml:space="preserve">38860</t>
   </si>
   <si>
+    <t xml:space="preserve">Portland</t>
+  </si>
+  <si>
     <t xml:space="preserve">Portland-South Portland</t>
   </si>
   <si>
-    <t xml:space="preserve">Portland</t>
-  </si>
-  <si>
     <t xml:space="preserve">ME</t>
   </si>
   <si>
@@ -287,12 +291,12 @@
     <t xml:space="preserve">39580</t>
   </si>
   <si>
+    <t xml:space="preserve">Raleigh</t>
+  </si>
+  <si>
     <t xml:space="preserve">Raleigh-Cary</t>
   </si>
   <si>
-    <t xml:space="preserve">Raleigh</t>
-  </si>
-  <si>
     <t xml:space="preserve">40060</t>
   </si>
   <si>
@@ -305,31 +309,667 @@
     <t xml:space="preserve">41700</t>
   </si>
   <si>
+    <t xml:space="preserve">San Antonio</t>
+  </si>
+  <si>
     <t xml:space="preserve">San Antonio-New Braunfels</t>
   </si>
   <si>
-    <t xml:space="preserve">San Antonio</t>
-  </si>
-  <si>
     <t xml:space="preserve">44060</t>
   </si>
   <si>
+    <t xml:space="preserve">Spokane</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spokane-Spokane Valley</t>
   </si>
   <si>
-    <t xml:space="preserve">Spokane</t>
-  </si>
-  <si>
     <t xml:space="preserve">WA</t>
   </si>
   <si>
     <t xml:space="preserve">49180</t>
   </si>
   <si>
+    <t xml:space="preserve">Winston</t>
+  </si>
+  <si>
     <t xml:space="preserve">Winston-Salem</t>
   </si>
   <si>
-    <t xml:space="preserve">Winston</t>
+    <t>msa</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>cbsa</t>
+  </si>
+  <si>
+    <t>rent_control</t>
+  </si>
+  <si>
+    <t>eviction_notice_days</t>
+  </si>
+  <si>
+    <t>security_deposit_limit</t>
+  </si>
+  <si>
+    <t>security_deposit_limit_num</t>
+  </si>
+  <si>
+    <t>n_eviction_notice</t>
+  </si>
+  <si>
+    <t>n_security_deposit</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>Huntsville</t>
+  </si>
+  <si>
+    <t>Fayetteville-Springdale-Rogers</t>
+  </si>
+  <si>
+    <t>Colorado Springs</t>
+  </si>
+  <si>
+    <t>Lakeland-Winter Haven</t>
+  </si>
+  <si>
+    <t>North Port-Sarasota-Bradenton</t>
+  </si>
+  <si>
+    <t>Palm Bay-Melbourne-Titusville</t>
+  </si>
+  <si>
+    <t>Pensacola-Ferry Pass-Brent</t>
+  </si>
+  <si>
+    <t>Port St. Lucie</t>
+  </si>
+  <si>
+    <t>Atlanta-Sandy Springs-Alpharetta</t>
+  </si>
+  <si>
+    <t>Augusta-Richmond County</t>
+  </si>
+  <si>
+    <t>Des Moines-West Des Moines</t>
+  </si>
+  <si>
+    <t>Indianapolis-Carmel-Anderson</t>
+  </si>
+  <si>
+    <t>Portland-South Portland</t>
+  </si>
+  <si>
+    <t>Fayetteville</t>
+  </si>
+  <si>
+    <t>Raleigh-Cary</t>
+  </si>
+  <si>
+    <t>Winston-Salem</t>
+  </si>
+  <si>
+    <t>Charlotte-Concord-Gastonia</t>
+  </si>
+  <si>
+    <t>Oklahoma City</t>
+  </si>
+  <si>
+    <t>Charleston-North Charleston</t>
+  </si>
+  <si>
+    <t>Columbia</t>
+  </si>
+  <si>
+    <t>Greenville-Anderson</t>
+  </si>
+  <si>
+    <t>Myrtle Beach-Conway-North Myrtle Beach</t>
+  </si>
+  <si>
+    <t>Knoxville</t>
+  </si>
+  <si>
+    <t>Nashville-Davidson--Murfreesboro--Franklin</t>
+  </si>
+  <si>
+    <t>Chattanooga</t>
+  </si>
+  <si>
+    <t>McAllen-Edinburg-Mission</t>
+  </si>
+  <si>
+    <t>San Antonio-New Braunfels</t>
+  </si>
+  <si>
+    <t>Richmond</t>
+  </si>
+  <si>
+    <t>Spokane-Spokane Valley</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>GA-SC</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>NC-SC</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SC-NC</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TN-GA</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>1_month_rent</t>
+  </si>
+  <si>
+    <t>2_months_rent</t>
+  </si>
+  <si>
+    <t>anchor_city</t>
+  </si>
+  <si>
+    <t>state.x</t>
+  </si>
+  <si>
+    <t>n_pop_growth</t>
+  </si>
+  <si>
+    <t>n_employ_change</t>
+  </si>
+  <si>
+    <t>n_occ_rate2021</t>
+  </si>
+  <si>
+    <t>n_rent_change</t>
+  </si>
+  <si>
+    <t>n_income_to_homeprice</t>
+  </si>
+  <si>
+    <t>n_rent_to_income</t>
+  </si>
+  <si>
+    <t>12060</t>
+  </si>
+  <si>
+    <t>12260</t>
+  </si>
+  <si>
+    <t>16700</t>
+  </si>
+  <si>
+    <t>16740</t>
+  </si>
+  <si>
+    <t>16860</t>
+  </si>
+  <si>
+    <t>17820</t>
+  </si>
+  <si>
+    <t>17900</t>
+  </si>
+  <si>
+    <t>19780</t>
+  </si>
+  <si>
+    <t>22180</t>
+  </si>
+  <si>
+    <t>22220</t>
+  </si>
+  <si>
+    <t>24860</t>
+  </si>
+  <si>
+    <t>26620</t>
+  </si>
+  <si>
+    <t>26900</t>
+  </si>
+  <si>
+    <t>28940</t>
+  </si>
+  <si>
+    <t>29460</t>
+  </si>
+  <si>
+    <t>32580</t>
+  </si>
+  <si>
+    <t>34820</t>
+  </si>
+  <si>
+    <t>34980</t>
+  </si>
+  <si>
+    <t>35840</t>
+  </si>
+  <si>
+    <t>36420</t>
+  </si>
+  <si>
+    <t>37340</t>
+  </si>
+  <si>
+    <t>37860</t>
+  </si>
+  <si>
+    <t>38860</t>
+  </si>
+  <si>
+    <t>38940</t>
+  </si>
+  <si>
+    <t>39580</t>
+  </si>
+  <si>
+    <t>40060</t>
+  </si>
+  <si>
+    <t>41700</t>
+  </si>
+  <si>
+    <t>44060</t>
+  </si>
+  <si>
+    <t>49180</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>Augusta</t>
+  </si>
+  <si>
+    <t>Charleston</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Des Moines</t>
+  </si>
+  <si>
+    <t>Greenville</t>
+  </si>
+  <si>
+    <t>Indianapolis</t>
+  </si>
+  <si>
+    <t>Lakeland</t>
+  </si>
+  <si>
+    <t>McAllen</t>
+  </si>
+  <si>
+    <t>Myrtle Beach</t>
+  </si>
+  <si>
+    <t>Nashville</t>
+  </si>
+  <si>
+    <t>Sarasota</t>
+  </si>
+  <si>
+    <t>Palm Bay</t>
+  </si>
+  <si>
+    <t>Pensacola</t>
+  </si>
+  <si>
+    <t>Portland</t>
+  </si>
+  <si>
+    <t>Raleigh</t>
+  </si>
+  <si>
+    <t>San Antonio</t>
+  </si>
+  <si>
+    <t>Spokane</t>
+  </si>
+  <si>
+    <t>Winston</t>
+  </si>
+  <si>
+    <t>stateabbrv</t>
+  </si>
+  <si>
+    <t>county.x</t>
+  </si>
+  <si>
+    <t>stcofips</t>
+  </si>
+  <si>
+    <t>risk_score</t>
+  </si>
+  <si>
+    <t>city_msa</t>
+  </si>
+  <si>
+    <t>n_climate_risk</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Cumberland</t>
+  </si>
+  <si>
+    <t>Polk</t>
+  </si>
+  <si>
+    <t>Brevard</t>
+  </si>
+  <si>
+    <t>Escambia</t>
+  </si>
+  <si>
+    <t>St. Lucie</t>
+  </si>
+  <si>
+    <t>Fulton</t>
+  </si>
+  <si>
+    <t>Marion</t>
+  </si>
+  <si>
+    <t>Forsyth</t>
+  </si>
+  <si>
+    <t>Mecklenburg</t>
+  </si>
+  <si>
+    <t>Wake</t>
+  </si>
+  <si>
+    <t>Horry</t>
+  </si>
+  <si>
+    <t>Richland</t>
+  </si>
+  <si>
+    <t>Davidson</t>
+  </si>
+  <si>
+    <t>Hamilton</t>
+  </si>
+  <si>
+    <t>Knox</t>
+  </si>
+  <si>
+    <t>Bexar</t>
+  </si>
+  <si>
+    <t>El Paso</t>
+  </si>
+  <si>
+    <t>Hidalgo</t>
+  </si>
+  <si>
+    <t>23005</t>
+  </si>
+  <si>
+    <t>19153</t>
+  </si>
+  <si>
+    <t>12009</t>
+  </si>
+  <si>
+    <t>12033</t>
+  </si>
+  <si>
+    <t>12105</t>
+  </si>
+  <si>
+    <t>12111</t>
+  </si>
+  <si>
+    <t>12115</t>
+  </si>
+  <si>
+    <t>13121</t>
+  </si>
+  <si>
+    <t>13245</t>
+  </si>
+  <si>
+    <t>18097</t>
+  </si>
+  <si>
+    <t>37051</t>
+  </si>
+  <si>
+    <t>37067</t>
+  </si>
+  <si>
+    <t>37119</t>
+  </si>
+  <si>
+    <t>37183</t>
+  </si>
+  <si>
+    <t>40109</t>
+  </si>
+  <si>
+    <t>45019</t>
+  </si>
+  <si>
+    <t>45045</t>
+  </si>
+  <si>
+    <t>45051</t>
+  </si>
+  <si>
+    <t>45079</t>
+  </si>
+  <si>
+    <t>47037</t>
+  </si>
+  <si>
+    <t>47065</t>
+  </si>
+  <si>
+    <t>47093</t>
+  </si>
+  <si>
+    <t>48029</t>
+  </si>
+  <si>
+    <t>48141</t>
+  </si>
+  <si>
+    <t>48215</t>
+  </si>
+  <si>
+    <t>51159</t>
+  </si>
+  <si>
+    <t>53063</t>
+  </si>
+  <si>
+    <t>1089</t>
+  </si>
+  <si>
+    <t>5143</t>
   </si>
 </sst>
 </file>
@@ -986,10 +1626,10 @@
         <v>41</v>
       </c>
       <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
         <v>42</v>
-      </c>
-      <c r="C11" t="s">
-        <v>39</v>
       </c>
       <c r="D11" t="s">
         <v>43</v>
@@ -1625,4 +2265,3826 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" t="n">
+        <v>26620.0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>194</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" t="n">
+        <v>22220.0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>195</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" t="n">
+        <v>17820.0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>192</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" t="n">
+        <v>29460.0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>192</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>192</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" t="n">
+        <v>35840.0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>192</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" t="n">
+        <v>37340.0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>192</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>192</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" t="n">
+        <v>37860.0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>192</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" t="n">
+        <v>38940.0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>192</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>192</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D10" t="n">
+        <v>12060.0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" t="s">
+        <v>178</v>
+      </c>
+      <c r="D11" t="n">
+        <v>12260.0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>192</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>192</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D12" t="n">
+        <v>19780.0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>195</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" t="n">
+        <v>26900.0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>192</v>
+      </c>
+      <c r="F13" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>192</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" t="s">
+        <v>181</v>
+      </c>
+      <c r="D14" t="n">
+        <v>38860.0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>193</v>
+      </c>
+      <c r="F14" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>195</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" t="n">
+        <v>22180.0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>192</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>195</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" t="s">
+        <v>182</v>
+      </c>
+      <c r="D16" t="n">
+        <v>39580.0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>192</v>
+      </c>
+      <c r="F16" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>195</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D17" t="n">
+        <v>49180.0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>192</v>
+      </c>
+      <c r="F17" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>195</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" t="s">
+        <v>183</v>
+      </c>
+      <c r="D18" t="n">
+        <v>16740.0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>192</v>
+      </c>
+      <c r="F18" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>195</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" t="n">
+        <v>36420.0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>192</v>
+      </c>
+      <c r="F19" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>192</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.6428571428571428</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" t="n">
+        <v>16700.0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>192</v>
+      </c>
+      <c r="F20" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>192</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.6428571428571428</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D21" t="n">
+        <v>17900.0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>192</v>
+      </c>
+      <c r="F21" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>192</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.6428571428571428</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22" t="n">
+        <v>24860.0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>192</v>
+      </c>
+      <c r="F22" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>192</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.6428571428571428</v>
+      </c>
+      <c r="J22" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D23" t="n">
+        <v>34820.0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>192</v>
+      </c>
+      <c r="F23" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>192</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.6428571428571428</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" t="s">
+        <v>187</v>
+      </c>
+      <c r="D24" t="n">
+        <v>28940.0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F24" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>192</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" t="s">
+        <v>187</v>
+      </c>
+      <c r="D25" t="n">
+        <v>34980.0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>192</v>
+      </c>
+      <c r="F25" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>192</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" t="s">
+        <v>188</v>
+      </c>
+      <c r="D26" t="n">
+        <v>16860.0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>192</v>
+      </c>
+      <c r="F26" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" t="n">
+        <v>32580.0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>192</v>
+      </c>
+      <c r="F27" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>192</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" t="s">
+        <v>170</v>
+      </c>
+      <c r="C28" t="s">
+        <v>189</v>
+      </c>
+      <c r="D28" t="n">
+        <v>41700.0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>192</v>
+      </c>
+      <c r="F28" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>192</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J28" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" t="s">
+        <v>171</v>
+      </c>
+      <c r="C29" t="s">
+        <v>190</v>
+      </c>
+      <c r="D29" t="n">
+        <v>40060.0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>192</v>
+      </c>
+      <c r="F29" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>195</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" t="s">
+        <v>191</v>
+      </c>
+      <c r="D30" t="n">
+        <v>44060.0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>192</v>
+      </c>
+      <c r="F30" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>192</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I1" t="s">
+        <v>201</v>
+      </c>
+      <c r="J1" t="s">
+        <v>202</v>
+      </c>
+      <c r="K1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.026904376012965952</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.5589796980739199</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.31007751937984407</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.462560289633494</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.5570947215131256</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.27061097190750283</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.02236628849270663</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.24627798021863614</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.29069767441860483</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.57480993002965</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.9147778978749298</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.3996891019116168</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" t="s">
+        <v>235</v>
+      </c>
+      <c r="E4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.206482982171799</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.37943779281624157</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.2713178294573629</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.7010918027783359</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.7064523935746643</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.08254139279902617</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.17990275526742303</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.44190525767829253</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.329457364341086</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.09946380416345772</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.42899023313340345</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.15660681365010565</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.03144246353322527</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.5317803227485685</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.49806201550387497</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.3693403452278073</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.9395807661796844</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.6210899426741521</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.06547811993517016</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.09945340968245706</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.48449612403100806</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.42398055396859263</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.1984999332926537</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.4680166823038622</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" t="s">
+        <v>185</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.09108589951377635</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.1446382092660073</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.2325581395348844</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.1625066424367611</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.6299748550891775</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.10988346623476541</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" t="s">
+        <v>237</v>
+      </c>
+      <c r="E9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.17763371150729335</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.10036439354502864</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.21317829457364246</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.26144161906140795</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.8140838382564638</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" t="s">
+        <v>182</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.06288492706645055</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.38196251952108284</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.25193798449612365</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.2915992029092922</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.7158187795413237</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.26954373942473087</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.4564019448946515</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.2066111400312337</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.57170542635659</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.5964805293615844</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.5094010152038302</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="s">
+        <v>214</v>
+      </c>
+      <c r="C12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" t="s">
+        <v>238</v>
+      </c>
+      <c r="E12" t="s">
+        <v>185</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.16888168557536468</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.3229047371160854</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.31007751937984407</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.3168680028194413</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.6429122309857133</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.2851823523808733</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C13" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" t="s">
+        <v>173</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.3705024311183144</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.42870900572618426</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.569767441860465</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.5792423426833726</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.3636090910207119</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.937218828313471</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" t="s">
+        <v>216</v>
+      </c>
+      <c r="C14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" t="s">
+        <v>239</v>
+      </c>
+      <c r="E14" t="s">
+        <v>180</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.658875585632483</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.2713178294573629</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.06860724103065555</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.5300990100603423</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.6381643106730985</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C15" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" t="s">
+        <v>166</v>
+      </c>
+      <c r="E15" t="s">
+        <v>187</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.23241491085899513</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.5036959916710047</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.7771317829457352</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.5065843967067801</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.6057490716156466</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.5476004559386869</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" t="s">
+        <v>218</v>
+      </c>
+      <c r="C16" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" t="s">
+        <v>240</v>
+      </c>
+      <c r="E16" t="s">
+        <v>176</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.8784440842787682</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.6763565891472862</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.30710433632700207</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.7582043477006727</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.17129944987938672</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" t="s">
+        <v>219</v>
+      </c>
+      <c r="C17" t="s">
+        <v>169</v>
+      </c>
+      <c r="D17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E17" t="s">
+        <v>189</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.1021069692058347</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.44747527329515885</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.5620155038759677</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.5584282999962582</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.39434008785007835</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" t="s">
+        <v>220</v>
+      </c>
+      <c r="C18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18" t="s">
+        <v>242</v>
+      </c>
+      <c r="E18" t="s">
+        <v>186</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.6425039042165539</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.5232558139534893</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.9329212188414181</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.3850938159843802</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C19" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" t="s">
+        <v>243</v>
+      </c>
+      <c r="E19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.07747163695299837</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.714679854242582</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.20736434108527013</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.39325024780865214</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.06277908050230296</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.16007457971458827</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" t="s">
+        <v>222</v>
+      </c>
+      <c r="C20" t="s">
+        <v>148</v>
+      </c>
+      <c r="D20" t="s">
+        <v>244</v>
+      </c>
+      <c r="E20" t="s">
+        <v>176</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.6761750405186385</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.7472149921915668</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.4903100775193804</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.45595200944311454</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.6133707099426824</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.15559927764132175</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" t="s">
+        <v>223</v>
+      </c>
+      <c r="C21" t="s">
+        <v>161</v>
+      </c>
+      <c r="D21" t="s">
+        <v>161</v>
+      </c>
+      <c r="E21" t="s">
+        <v>184</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.0927066450567261</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.4646277980218636</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.1099079881948337</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.6508117737883212</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.5193941214342297</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" t="s">
+        <v>224</v>
+      </c>
+      <c r="C22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D22" t="s">
+        <v>245</v>
+      </c>
+      <c r="E22" t="s">
+        <v>176</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.25867098865478116</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.6409942738157209</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.569767441860465</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.38464512749300483</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.739095205322849</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.21209380667798994</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" t="s">
+        <v>225</v>
+      </c>
+      <c r="C23" t="s">
+        <v>150</v>
+      </c>
+      <c r="D23" t="s">
+        <v>246</v>
+      </c>
+      <c r="E23" t="s">
+        <v>176</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.10502431118314423</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.4690265486725664</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.6007751937984489</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.27523346702722457</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.8974810020096098</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.35630390723791416</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" t="s">
+        <v>226</v>
+      </c>
+      <c r="C24" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" t="s">
+        <v>247</v>
+      </c>
+      <c r="E24" t="s">
+        <v>181</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.08103727714748785</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.690161374284227</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.5505497254799816</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.726882758275447</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C25" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" t="s">
+        <v>151</v>
+      </c>
+      <c r="E25" t="s">
+        <v>176</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.706969205834684</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.1356589147286828</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.33147597254875977</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.7800336626165053</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.11240179631878333</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" t="s">
+        <v>228</v>
+      </c>
+      <c r="C26" t="s">
+        <v>158</v>
+      </c>
+      <c r="D26" t="s">
+        <v>248</v>
+      </c>
+      <c r="E26" t="s">
+        <v>182</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.4424635332252837</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.37160333159812603</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.34883720930232526</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.14206845699364085</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.37315160687749427</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.43780960005691505</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C27" t="s">
+        <v>171</v>
+      </c>
+      <c r="D27" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" t="s">
+        <v>190</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.004213938411669372</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.44856845393024475</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.39728682170542606</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.1489893320435514</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.7494641064616268</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.23009952776360565</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" t="s">
+        <v>230</v>
+      </c>
+      <c r="C28" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" t="s">
+        <v>249</v>
+      </c>
+      <c r="E28" t="s">
+        <v>189</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.24246353322528366</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.3723841749089016</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.48449612403100806</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.3272050392920731</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.4093495033156547</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.246083616286774</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" t="s">
+        <v>231</v>
+      </c>
+      <c r="C29" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" t="s">
+        <v>250</v>
+      </c>
+      <c r="E29" t="s">
+        <v>191</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.14132901134521883</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.5755075481520042</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.8914728682170537</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.17996109190105342</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.6159439732445982</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.5383954685370023</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" t="s">
+        <v>232</v>
+      </c>
+      <c r="C30" t="s">
+        <v>159</v>
+      </c>
+      <c r="D30" t="s">
+        <v>251</v>
+      </c>
+      <c r="E30" t="s">
+        <v>182</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.04181523500810373</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.40827693909422175</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.42635658914728763</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.6446897733958128</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.5596334787079904</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" t="n">
+        <v>26620.0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>194</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" t="n">
+        <v>22220.0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>195</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" t="n">
+        <v>17820.0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>192</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>192</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" t="n">
+        <v>29460.0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>192</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>192</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" t="n">
+        <v>35840.0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>192</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" t="n">
+        <v>37340.0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>192</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>192</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" t="n">
+        <v>37860.0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>192</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" t="n">
+        <v>38940.0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>192</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>192</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D10" t="n">
+        <v>12060.0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>192</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" t="s">
+        <v>178</v>
+      </c>
+      <c r="D11" t="n">
+        <v>12260.0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>192</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>192</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D12" t="n">
+        <v>19780.0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>195</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" t="n">
+        <v>26900.0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>192</v>
+      </c>
+      <c r="F13" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>192</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" t="s">
+        <v>181</v>
+      </c>
+      <c r="D14" t="n">
+        <v>38860.0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>193</v>
+      </c>
+      <c r="F14" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>195</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" t="n">
+        <v>22180.0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>192</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>195</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" t="s">
+        <v>182</v>
+      </c>
+      <c r="D16" t="n">
+        <v>39580.0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>192</v>
+      </c>
+      <c r="F16" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>195</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D17" t="n">
+        <v>49180.0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>192</v>
+      </c>
+      <c r="F17" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>195</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" t="s">
+        <v>183</v>
+      </c>
+      <c r="D18" t="n">
+        <v>16740.0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>192</v>
+      </c>
+      <c r="F18" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>195</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" t="n">
+        <v>36420.0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>192</v>
+      </c>
+      <c r="F19" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>192</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.6428571428571428</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" t="n">
+        <v>16700.0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>192</v>
+      </c>
+      <c r="F20" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>192</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.6428571428571428</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D21" t="n">
+        <v>17900.0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>192</v>
+      </c>
+      <c r="F21" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>192</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.6428571428571428</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22" t="n">
+        <v>24860.0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>192</v>
+      </c>
+      <c r="F22" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>192</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.6428571428571428</v>
+      </c>
+      <c r="J22" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D23" t="n">
+        <v>34820.0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>192</v>
+      </c>
+      <c r="F23" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>192</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.6428571428571428</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" t="s">
+        <v>187</v>
+      </c>
+      <c r="D24" t="n">
+        <v>28940.0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F24" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>192</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" t="s">
+        <v>187</v>
+      </c>
+      <c r="D25" t="n">
+        <v>34980.0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>192</v>
+      </c>
+      <c r="F25" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>192</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" t="s">
+        <v>188</v>
+      </c>
+      <c r="D26" t="n">
+        <v>16860.0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>192</v>
+      </c>
+      <c r="F26" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>192</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" t="n">
+        <v>32580.0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>192</v>
+      </c>
+      <c r="F27" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>192</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" t="s">
+        <v>170</v>
+      </c>
+      <c r="C28" t="s">
+        <v>189</v>
+      </c>
+      <c r="D28" t="n">
+        <v>41700.0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>192</v>
+      </c>
+      <c r="F28" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>192</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="J28" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" t="s">
+        <v>171</v>
+      </c>
+      <c r="C29" t="s">
+        <v>190</v>
+      </c>
+      <c r="D29" t="n">
+        <v>40060.0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>192</v>
+      </c>
+      <c r="F29" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>195</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" t="s">
+        <v>191</v>
+      </c>
+      <c r="D30" t="n">
+        <v>44060.0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>192</v>
+      </c>
+      <c r="F30" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>192</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" t="s">
+        <v>256</v>
+      </c>
+      <c r="I1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F2" t="n">
+        <v>9.805792966460626</v>
+      </c>
+      <c r="G2" t="n">
+        <v>38860.0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>247</v>
+      </c>
+      <c r="I2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E3" t="s">
+        <v>290</v>
+      </c>
+      <c r="F3" t="n">
+        <v>15.206695345283824</v>
+      </c>
+      <c r="G3" t="n">
+        <v>19780.0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>237</v>
+      </c>
+      <c r="I3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F4" t="n">
+        <v>30.218700714391023</v>
+      </c>
+      <c r="G4" t="n">
+        <v>37340.0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>245</v>
+      </c>
+      <c r="I4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" t="s">
+        <v>274</v>
+      </c>
+      <c r="E5" t="s">
+        <v>292</v>
+      </c>
+      <c r="F5" t="n">
+        <v>27.162830286749713</v>
+      </c>
+      <c r="G5" t="n">
+        <v>37860.0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>246</v>
+      </c>
+      <c r="I5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>260</v>
+      </c>
+      <c r="C6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" t="s">
+        <v>272</v>
+      </c>
+      <c r="E6" t="s">
+        <v>293</v>
+      </c>
+      <c r="F6" t="n">
+        <v>28.92348693485065</v>
+      </c>
+      <c r="G6" t="n">
+        <v>29460.0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>240</v>
+      </c>
+      <c r="I6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" t="s">
+        <v>275</v>
+      </c>
+      <c r="E7" t="s">
+        <v>294</v>
+      </c>
+      <c r="F7" t="n">
+        <v>41.930238616014215</v>
+      </c>
+      <c r="G7" t="n">
+        <v>38940.0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>151</v>
+      </c>
+      <c r="I7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" t="s">
+        <v>244</v>
+      </c>
+      <c r="E8" t="s">
+        <v>295</v>
+      </c>
+      <c r="F8" t="n">
+        <v>24.18572155105568</v>
+      </c>
+      <c r="G8" t="n">
+        <v>35840.0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>244</v>
+      </c>
+      <c r="I8"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" t="s">
+        <v>276</v>
+      </c>
+      <c r="E9" t="s">
+        <v>296</v>
+      </c>
+      <c r="F9" t="n">
+        <v>16.312105093906517</v>
+      </c>
+      <c r="G9" t="n">
+        <v>12060.0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>233</v>
+      </c>
+      <c r="I9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>261</v>
+      </c>
+      <c r="C10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E10" t="s">
+        <v>297</v>
+      </c>
+      <c r="F10" t="n">
+        <v>19.551030060523985</v>
+      </c>
+      <c r="G10" t="n">
+        <v>12260.0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" t="s">
+        <v>262</v>
+      </c>
+      <c r="C11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D11" t="s">
+        <v>277</v>
+      </c>
+      <c r="E11" t="s">
+        <v>298</v>
+      </c>
+      <c r="F11" t="n">
+        <v>22.21710935540322</v>
+      </c>
+      <c r="G11" t="n">
+        <v>26900.0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>239</v>
+      </c>
+      <c r="I11"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="s">
+        <v>263</v>
+      </c>
+      <c r="C12" t="s">
+        <v>182</v>
+      </c>
+      <c r="D12" t="s">
+        <v>271</v>
+      </c>
+      <c r="E12" t="s">
+        <v>299</v>
+      </c>
+      <c r="F12" t="n">
+        <v>17.744000976788264</v>
+      </c>
+      <c r="G12" t="n">
+        <v>22180.0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>157</v>
+      </c>
+      <c r="I12"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" t="s">
+        <v>263</v>
+      </c>
+      <c r="C13" t="s">
+        <v>182</v>
+      </c>
+      <c r="D13" t="s">
+        <v>278</v>
+      </c>
+      <c r="E13" t="s">
+        <v>300</v>
+      </c>
+      <c r="F13" t="n">
+        <v>16.747941254315975</v>
+      </c>
+      <c r="G13" t="n">
+        <v>49180.0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>251</v>
+      </c>
+      <c r="I13"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C14" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" t="s">
+        <v>279</v>
+      </c>
+      <c r="E14" t="s">
+        <v>301</v>
+      </c>
+      <c r="F14" t="n">
+        <v>16.368428591765817</v>
+      </c>
+      <c r="G14" t="n">
+        <v>16740.0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>236</v>
+      </c>
+      <c r="I14"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" t="s">
+        <v>280</v>
+      </c>
+      <c r="E15" t="s">
+        <v>302</v>
+      </c>
+      <c r="F15" t="n">
+        <v>11.750802543446456</v>
+      </c>
+      <c r="G15" t="n">
+        <v>39580.0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>248</v>
+      </c>
+      <c r="I15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" t="s">
+        <v>264</v>
+      </c>
+      <c r="C16" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" t="s">
+        <v>264</v>
+      </c>
+      <c r="E16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F16" t="n">
+        <v>32.51090968732113</v>
+      </c>
+      <c r="G16" t="n">
+        <v>36420.0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>161</v>
+      </c>
+      <c r="I16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C17" t="s">
+        <v>185</v>
+      </c>
+      <c r="D17" t="s">
+        <v>235</v>
+      </c>
+      <c r="E17" t="s">
+        <v>304</v>
+      </c>
+      <c r="F17" t="n">
+        <v>25.035971607427683</v>
+      </c>
+      <c r="G17" t="n">
+        <v>16700.0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>235</v>
+      </c>
+      <c r="I17"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" t="s">
+        <v>265</v>
+      </c>
+      <c r="C18" t="s">
+        <v>185</v>
+      </c>
+      <c r="D18" t="s">
+        <v>238</v>
+      </c>
+      <c r="E18" t="s">
+        <v>305</v>
+      </c>
+      <c r="F18" t="n">
+        <v>15.117283646908604</v>
+      </c>
+      <c r="G18" t="n">
+        <v>24860.0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>238</v>
+      </c>
+      <c r="I18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" t="s">
+        <v>265</v>
+      </c>
+      <c r="C19" t="s">
+        <v>185</v>
+      </c>
+      <c r="D19" t="s">
+        <v>281</v>
+      </c>
+      <c r="E19" t="s">
+        <v>306</v>
+      </c>
+      <c r="F19" t="n">
+        <v>26.24959195922409</v>
+      </c>
+      <c r="G19" t="n">
+        <v>34820.0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>242</v>
+      </c>
+      <c r="I19"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" t="s">
+        <v>265</v>
+      </c>
+      <c r="C20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" t="s">
+        <v>282</v>
+      </c>
+      <c r="E20" t="s">
+        <v>307</v>
+      </c>
+      <c r="F20" t="n">
+        <v>17.58532201739729</v>
+      </c>
+      <c r="G20" t="n">
+        <v>17900.0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>163</v>
+      </c>
+      <c r="I20"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" t="s">
+        <v>266</v>
+      </c>
+      <c r="C21" t="s">
+        <v>187</v>
+      </c>
+      <c r="D21" t="s">
+        <v>283</v>
+      </c>
+      <c r="E21" t="s">
+        <v>308</v>
+      </c>
+      <c r="F21" t="n">
+        <v>28.296548389730063</v>
+      </c>
+      <c r="G21" t="n">
+        <v>34980.0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>243</v>
+      </c>
+      <c r="I21"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" t="s">
+        <v>266</v>
+      </c>
+      <c r="C22" t="s">
+        <v>187</v>
+      </c>
+      <c r="D22" t="s">
+        <v>284</v>
+      </c>
+      <c r="E22" t="s">
+        <v>309</v>
+      </c>
+      <c r="F22" t="n">
+        <v>20.757475846420267</v>
+      </c>
+      <c r="G22" t="n">
+        <v>16860.0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>168</v>
+      </c>
+      <c r="I22"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" t="s">
+        <v>266</v>
+      </c>
+      <c r="C23" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23" t="s">
+        <v>285</v>
+      </c>
+      <c r="E23" t="s">
+        <v>310</v>
+      </c>
+      <c r="F23" t="n">
+        <v>15.650793173410102</v>
+      </c>
+      <c r="G23" t="n">
+        <v>28940.0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>166</v>
+      </c>
+      <c r="I23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" t="s">
+        <v>267</v>
+      </c>
+      <c r="C24" t="s">
+        <v>189</v>
+      </c>
+      <c r="D24" t="s">
+        <v>286</v>
+      </c>
+      <c r="E24" t="s">
+        <v>311</v>
+      </c>
+      <c r="F24" t="n">
+        <v>39.952943339570595</v>
+      </c>
+      <c r="G24" t="n">
+        <v>41700.0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>249</v>
+      </c>
+      <c r="I24"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" t="s">
+        <v>267</v>
+      </c>
+      <c r="C25" t="s">
+        <v>189</v>
+      </c>
+      <c r="D25" t="s">
+        <v>287</v>
+      </c>
+      <c r="E25" t="s">
+        <v>312</v>
+      </c>
+      <c r="F25" t="n">
+        <v>35.67096512100983</v>
+      </c>
+      <c r="G25" t="n">
+        <v>17820.0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>146</v>
+      </c>
+      <c r="I25"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" t="s">
+        <v>267</v>
+      </c>
+      <c r="C26" t="s">
+        <v>189</v>
+      </c>
+      <c r="D26" t="s">
+        <v>288</v>
+      </c>
+      <c r="E26" t="s">
+        <v>313</v>
+      </c>
+      <c r="F26" t="n">
+        <v>38.061258729011314</v>
+      </c>
+      <c r="G26" t="n">
+        <v>32580.0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>241</v>
+      </c>
+      <c r="I26"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" t="s">
+        <v>268</v>
+      </c>
+      <c r="C27" t="s">
+        <v>190</v>
+      </c>
+      <c r="D27" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" t="s">
+        <v>314</v>
+      </c>
+      <c r="F27" t="n">
+        <v>4.701154273844042</v>
+      </c>
+      <c r="G27" t="n">
+        <v>40060.0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>171</v>
+      </c>
+      <c r="I27"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" t="s">
+        <v>269</v>
+      </c>
+      <c r="C28" t="s">
+        <v>191</v>
+      </c>
+      <c r="D28" t="s">
+        <v>250</v>
+      </c>
+      <c r="E28" t="s">
+        <v>315</v>
+      </c>
+      <c r="F28" t="n">
+        <v>11.898868598083514</v>
+      </c>
+      <c r="G28" t="n">
+        <v>44060.0</v>
+      </c>
+      <c r="H28" t="s">
+        <v>250</v>
+      </c>
+      <c r="I28"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" t="s">
+        <v>270</v>
+      </c>
+      <c r="C29" t="s">
+        <v>270</v>
+      </c>
+      <c r="D29" t="s">
+        <v>270</v>
+      </c>
+      <c r="E29" t="s">
+        <v>316</v>
+      </c>
+      <c r="F29"/>
+      <c r="G29" t="n">
+        <v>26620.0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>144</v>
+      </c>
+      <c r="I29"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" t="s">
+        <v>270</v>
+      </c>
+      <c r="C30" t="s">
+        <v>270</v>
+      </c>
+      <c r="D30" t="s">
+        <v>270</v>
+      </c>
+      <c r="E30" t="s">
+        <v>317</v>
+      </c>
+      <c r="F30"/>
+      <c r="G30" t="n">
+        <v>22220.0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>157</v>
+      </c>
+      <c r="I30"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>